<commit_message>
Re-organize packages and edit code
</commit_message>
<xml_diff>
--- a/Template_Import_Sustenance.xlsx
+++ b/Template_Import_Sustenance.xlsx
@@ -56,9 +56,6 @@
     <t>Milk</t>
   </si>
   <si>
-    <t>Type (Select)</t>
-  </si>
-  <si>
     <t>Type ID</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Strawberry Soda</t>
+  </si>
+  <si>
+    <t>Type ID (Select)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +502,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="5">
         <v>1</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>30000</v>
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>4</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>32000</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>28000</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>30000</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>28000</v>
@@ -633,7 +633,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tIyhLGXM4xwo5T8jJpIsHPAIlQxULmo0yQ8eRcXImNT/pDKJifjdA4fpnYJ5W61IddKYNxnfltLdoCFl1I3wNg==" saltValue="qNba4Uy4gdlo+yeyNtpFAQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="a2CfDR3jZbPbc5m2Gy8TP0lRGieP+QKLw82swfBbFJi4k1iAAEocDtbrKNivQq5ph2jOJ4B4119hMfsSZR3mRQ==" saltValue="ZIm2JiE0A/LCFWzoU1LWvg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D6">
       <formula1>ISNUMBER(B2)</formula1>

</xml_diff>